<commit_message>
move october stations weather data in single file
</commit_message>
<xml_diff>
--- a/Lancaster University Project Folder/Data for Weather Project/NR Weather Stations/All NR NW&C Weather Stations.xlsx
+++ b/Lancaster University Project Folder/Data for Weather Project/NR Weather Stations/All NR NW&C Weather Stations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hayley.bull\Box\Lancaster University Project Folder\Data for Weather Project\NR Weather Stations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Notes\DSF Project\WeatherPerformanceProject\Lancaster University Project Folder\Data for Weather Project\NR Weather Stations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB27B5A4-7E39-40F9-AD16-F4AFDA885301}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D84B4F-8C98-4177-9899-BFBA30FA9930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{42A78A84-E7A4-4B9E-8DB5-9DBAC699443E}"/>
+    <workbookView xWindow="5892" yWindow="4128" windowWidth="17280" windowHeight="9072" xr2:uid="{42A78A84-E7A4-4B9E-8DB5-9DBAC699443E}"/>
   </bookViews>
   <sheets>
     <sheet name="Weather Stations" sheetId="1" r:id="rId1"/>
@@ -2117,9 +2117,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2133,9 +2130,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2174,9 +2168,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2251,9 +2242,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2303,9 +2291,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2331,9 +2316,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2387,16 +2369,10 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2427,9 +2403,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2438,18 +2411,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="29" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2505,6 +2472,39 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2908,25 +2908,25 @@
   <dimension ref="A1:M68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.33203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.88671875" style="29" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" style="29" customWidth="1"/>
+    <col min="2" max="2" width="43.88671875" style="28" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" style="28" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" style="10" customWidth="1"/>
     <col min="5" max="5" width="12.5546875" style="10" customWidth="1"/>
     <col min="6" max="6" width="14.5546875" style="10" customWidth="1"/>
-    <col min="7" max="7" width="18.88671875" style="29" customWidth="1"/>
-    <col min="8" max="8" width="104.88671875" style="29" customWidth="1"/>
-    <col min="9" max="9" width="30.5546875" style="29" customWidth="1"/>
-    <col min="10" max="10" width="28.5546875" style="29" customWidth="1"/>
-    <col min="11" max="11" width="20.109375" style="29" customWidth="1"/>
+    <col min="7" max="7" width="18.88671875" style="28" customWidth="1"/>
+    <col min="8" max="8" width="104.88671875" style="28" customWidth="1"/>
+    <col min="9" max="9" width="30.5546875" style="28" customWidth="1"/>
+    <col min="10" max="10" width="28.5546875" style="28" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" style="28" customWidth="1"/>
     <col min="12" max="12" width="18.5546875" style="10" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="26.33203125" style="10" customWidth="1"/>
-    <col min="14" max="16384" width="9.109375" style="29"/>
+    <col min="14" max="16384" width="9.109375" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="10" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3038,13 +3038,13 @@
       <c r="J3" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="K3" s="179" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="M3" s="28" t="s">
+      <c r="L3" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="27" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3061,10 +3061,10 @@
       <c r="D4" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="29">
         <v>35</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="30" t="s">
         <v>31</v>
       </c>
       <c r="G4" s="20" t="s">
@@ -3076,19 +3076,19 @@
       <c r="I4" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="32" t="s">
+      <c r="J4" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="33"/>
-      <c r="L4" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="M4" s="28" t="s">
+      <c r="K4" s="171"/>
+      <c r="L4" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="27" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="28.2" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="34">
+      <c r="A5" s="32">
         <v>14</v>
       </c>
       <c r="B5" s="19" t="s">
@@ -3097,13 +3097,13 @@
       <c r="C5" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="36">
+      <c r="E5" s="34">
         <v>4</v>
       </c>
-      <c r="F5" s="37">
+      <c r="F5" s="35">
         <v>1584</v>
       </c>
       <c r="G5" s="20" t="s">
@@ -3115,49 +3115,49 @@
       <c r="I5" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="38" t="s">
+      <c r="J5" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="K5" s="33"/>
-      <c r="L5" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="M5" s="39" t="s">
+      <c r="K5" s="171"/>
+      <c r="L5" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" s="37" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="40">
+      <c r="A6" s="38">
         <v>54</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="43" t="s">
+      <c r="D6" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="43">
+      <c r="E6" s="41">
         <v>82</v>
       </c>
-      <c r="F6" s="44" t="s">
+      <c r="F6" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="42" t="s">
+      <c r="G6" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="42" t="s">
+      <c r="H6" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="I6" s="45" t="s">
+      <c r="I6" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="46" t="s">
+      <c r="J6" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="K6" s="47" t="s">
+      <c r="K6" s="169" t="s">
         <v>47</v>
       </c>
       <c r="L6" s="17" t="s">
@@ -3195,14 +3195,14 @@
       <c r="I7" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="J7" s="32" t="s">
+      <c r="J7" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="33"/>
-      <c r="L7" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="M7" s="48" t="s">
+      <c r="K7" s="171"/>
+      <c r="L7" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" s="45" t="s">
         <v>35</v>
       </c>
     </row>
@@ -3216,13 +3216,13 @@
       <c r="C8" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="49" t="s">
+      <c r="D8" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="50">
+      <c r="E8" s="47">
         <v>46</v>
       </c>
-      <c r="F8" s="51">
+      <c r="F8" s="48">
         <v>1298</v>
       </c>
       <c r="G8" s="20" t="s">
@@ -3234,14 +3234,14 @@
       <c r="I8" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="J8" s="38" t="s">
+      <c r="J8" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="K8" s="33"/>
-      <c r="L8" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="M8" s="52" t="s">
+      <c r="K8" s="171"/>
+      <c r="L8" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="49" t="s">
         <v>35</v>
       </c>
     </row>
@@ -3249,32 +3249,32 @@
       <c r="A9" s="18">
         <v>58</v>
       </c>
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="55" t="s">
+      <c r="D9" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="56">
+      <c r="E9" s="53">
         <v>67</v>
       </c>
-      <c r="F9" s="57" t="s">
+      <c r="F9" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="G9" s="58" t="s">
+      <c r="G9" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="H9" s="59" t="s">
+      <c r="H9" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="I9" s="60" t="s">
+      <c r="I9" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="J9" s="61"/>
-      <c r="K9" s="47" t="s">
+      <c r="J9" s="58"/>
+      <c r="K9" s="169" t="s">
         <v>63</v>
       </c>
       <c r="L9" s="17" t="s">
@@ -3306,18 +3306,18 @@
       <c r="G10" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="H10" s="62" t="s">
+      <c r="H10" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="I10" s="63" t="s">
+      <c r="I10" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="J10" s="32"/>
-      <c r="K10" s="33"/>
-      <c r="L10" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="M10" s="48" t="s">
+      <c r="J10" s="31"/>
+      <c r="K10" s="171"/>
+      <c r="L10" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" s="45" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3325,19 +3325,19 @@
       <c r="A11" s="18">
         <v>9</v>
       </c>
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="61" t="s">
         <v>68</v>
       </c>
       <c r="C11" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="65" t="s">
+      <c r="D11" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="E11" s="66">
+      <c r="E11" s="63">
         <v>94</v>
       </c>
-      <c r="F11" s="67">
+      <c r="F11" s="64">
         <v>1650</v>
       </c>
       <c r="G11" s="20" t="s">
@@ -3349,12 +3349,12 @@
       <c r="I11" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="J11" s="32"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="M11" s="48" t="s">
+      <c r="J11" s="31"/>
+      <c r="K11" s="171"/>
+      <c r="L11" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="M11" s="45" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3362,36 +3362,36 @@
       <c r="A12" s="18">
         <v>53</v>
       </c>
-      <c r="B12" s="68" t="s">
+      <c r="B12" s="65" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="69" t="s">
+      <c r="C12" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="70" t="s">
+      <c r="D12" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="71">
+      <c r="E12" s="68">
         <v>56</v>
       </c>
-      <c r="F12" s="72">
+      <c r="F12" s="69">
         <v>1339</v>
       </c>
-      <c r="G12" s="73" t="s">
+      <c r="G12" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="74" t="s">
+      <c r="H12" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="I12" s="75" t="s">
+      <c r="I12" s="72" t="s">
         <v>75</v>
       </c>
-      <c r="J12" s="76"/>
-      <c r="K12" s="77"/>
-      <c r="L12" s="78" t="s">
-        <v>19</v>
-      </c>
-      <c r="M12" s="78" t="s">
+      <c r="J12" s="73"/>
+      <c r="K12" s="172"/>
+      <c r="L12" s="74" t="s">
+        <v>19</v>
+      </c>
+      <c r="M12" s="74" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3399,40 +3399,40 @@
       <c r="A13" s="18">
         <v>63</v>
       </c>
-      <c r="B13" s="53" t="s">
+      <c r="B13" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="54" t="s">
+      <c r="C13" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="55" t="s">
+      <c r="D13" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="E13" s="56">
+      <c r="E13" s="53">
         <v>0</v>
       </c>
-      <c r="F13" s="57" t="s">
+      <c r="F13" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="G13" s="58" t="s">
+      <c r="G13" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="H13" s="54" t="s">
+      <c r="H13" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="I13" s="79" t="s">
+      <c r="I13" s="75" t="s">
         <v>80</v>
       </c>
-      <c r="J13" s="46" t="s">
+      <c r="J13" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="K13" s="47" t="s">
+      <c r="K13" s="169" t="s">
         <v>82</v>
       </c>
-      <c r="L13" s="80" t="s">
-        <v>19</v>
-      </c>
-      <c r="M13" s="80" t="s">
+      <c r="L13" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="M13" s="76" t="s">
         <v>35</v>
       </c>
     </row>
@@ -3440,19 +3440,19 @@
       <c r="A14" s="18">
         <v>19</v>
       </c>
-      <c r="B14" s="64" t="s">
+      <c r="B14" s="61" t="s">
         <v>83</v>
       </c>
       <c r="C14" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="65" t="s">
+      <c r="D14" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="E14" s="66">
+      <c r="E14" s="63">
         <v>8</v>
       </c>
-      <c r="F14" s="67" t="s">
+      <c r="F14" s="64" t="s">
         <v>85</v>
       </c>
       <c r="G14" s="20" t="s">
@@ -3464,14 +3464,14 @@
       <c r="I14" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="J14" s="32" t="s">
+      <c r="J14" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="K14" s="33"/>
-      <c r="L14" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="M14" s="48" t="s">
+      <c r="K14" s="171"/>
+      <c r="L14" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="M14" s="45" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3479,10 +3479,10 @@
       <c r="A15" s="18">
         <v>17</v>
       </c>
-      <c r="B15" s="81" t="s">
+      <c r="B15" s="77" t="s">
         <v>88</v>
       </c>
-      <c r="C15" s="82" t="s">
+      <c r="C15" s="78" t="s">
         <v>29</v>
       </c>
       <c r="D15" s="21" t="s">
@@ -3491,71 +3491,71 @@
       <c r="E15" s="21">
         <v>30</v>
       </c>
-      <c r="F15" s="83" t="s">
+      <c r="F15" s="79" t="s">
         <v>90</v>
       </c>
-      <c r="G15" s="84" t="s">
+      <c r="G15" s="80" t="s">
         <v>91</v>
       </c>
-      <c r="H15" s="82" t="s">
+      <c r="H15" s="78" t="s">
         <v>92</v>
       </c>
-      <c r="I15" s="63" t="s">
+      <c r="I15" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="J15" s="63" t="s">
+      <c r="J15" s="60" t="s">
         <v>94</v>
       </c>
-      <c r="K15" s="33"/>
-      <c r="L15" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="M15" s="48" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="14.4" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K15" s="171"/>
+      <c r="L15" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="M15" s="45" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18">
         <v>52</v>
       </c>
-      <c r="B16" s="85" t="s">
+      <c r="B16" s="81" t="s">
         <v>95</v>
       </c>
-      <c r="C16" s="86" t="s">
+      <c r="C16" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="87" t="s">
+      <c r="D16" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="88">
+      <c r="E16" s="84">
         <v>37</v>
       </c>
-      <c r="F16" s="89" t="s">
+      <c r="F16" s="85" t="s">
         <v>96</v>
       </c>
-      <c r="G16" s="90" t="s">
+      <c r="G16" s="86" t="s">
         <v>43</v>
       </c>
-      <c r="H16" s="86" t="s">
+      <c r="H16" s="82" t="s">
         <v>97</v>
       </c>
-      <c r="I16" s="91" t="s">
+      <c r="I16" s="87" t="s">
         <v>98</v>
       </c>
       <c r="J16" s="26"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="M16" s="52" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="14.4" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K16" s="171"/>
+      <c r="L16" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="M16" s="49" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18">
         <v>62</v>
       </c>
-      <c r="B17" s="92" t="s">
+      <c r="B17" s="88" t="s">
         <v>99</v>
       </c>
       <c r="C17" s="20" t="s">
@@ -3579,92 +3579,92 @@
       <c r="I17" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="J17" s="32"/>
-      <c r="K17" s="27" t="s">
+      <c r="J17" s="31"/>
+      <c r="K17" s="179" t="s">
         <v>103</v>
       </c>
-      <c r="L17" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="M17" s="48" t="s">
+      <c r="L17" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="M17" s="45" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="14.4" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="34">
+      <c r="A18" s="32">
         <v>67</v>
       </c>
-      <c r="B18" s="93" t="s">
+      <c r="B18" s="89" t="s">
         <v>104</v>
       </c>
-      <c r="C18" s="69" t="s">
+      <c r="C18" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="70" t="s">
+      <c r="D18" s="67" t="s">
         <v>105</v>
       </c>
-      <c r="E18" s="71">
+      <c r="E18" s="68">
         <v>5</v>
       </c>
-      <c r="F18" s="72">
+      <c r="F18" s="69">
         <v>1440</v>
       </c>
-      <c r="G18" s="73" t="s">
+      <c r="G18" s="70" t="s">
         <v>106</v>
       </c>
-      <c r="H18" s="69" t="s">
+      <c r="H18" s="66" t="s">
         <v>107</v>
       </c>
-      <c r="I18" s="94" t="s">
+      <c r="I18" s="90" t="s">
         <v>108</v>
       </c>
-      <c r="J18" s="76"/>
-      <c r="K18" s="77"/>
-      <c r="L18" s="78" t="s">
-        <v>19</v>
-      </c>
-      <c r="M18" s="78" t="s">
+      <c r="J18" s="73"/>
+      <c r="K18" s="172"/>
+      <c r="L18" s="74" t="s">
+        <v>19</v>
+      </c>
+      <c r="M18" s="74" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A19" s="40">
+      <c r="A19" s="38">
         <v>44</v>
       </c>
-      <c r="B19" s="95" t="s">
+      <c r="B19" s="91" t="s">
         <v>109</v>
       </c>
-      <c r="C19" s="54" t="s">
+      <c r="C19" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="96" t="s">
+      <c r="D19" s="92" t="s">
         <v>110</v>
       </c>
-      <c r="E19" s="56">
+      <c r="E19" s="53">
         <v>35</v>
       </c>
-      <c r="F19" s="57" t="s">
+      <c r="F19" s="54" t="s">
         <v>111</v>
       </c>
-      <c r="G19" s="54" t="s">
+      <c r="G19" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="H19" s="54" t="s">
+      <c r="H19" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="I19" s="79" t="s">
+      <c r="I19" s="75" t="s">
         <v>114</v>
       </c>
-      <c r="J19" s="61" t="s">
+      <c r="J19" s="58" t="s">
         <v>115</v>
       </c>
-      <c r="K19" s="47" t="s">
+      <c r="K19" s="169" t="s">
         <v>116</v>
       </c>
-      <c r="L19" s="80" t="s">
-        <v>19</v>
-      </c>
-      <c r="M19" s="80" t="s">
+      <c r="L19" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="M19" s="76" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3672,13 +3672,13 @@
       <c r="A20" s="18">
         <v>45</v>
       </c>
-      <c r="B20" s="97" t="s">
+      <c r="B20" s="93" t="s">
         <v>117</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="98" t="s">
+      <c r="D20" s="94" t="s">
         <v>110</v>
       </c>
       <c r="E20" s="22">
@@ -3696,12 +3696,12 @@
       <c r="I20" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="J20" s="32"/>
-      <c r="K20" s="99"/>
-      <c r="L20" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="M20" s="48" t="s">
+      <c r="J20" s="31"/>
+      <c r="K20" s="170"/>
+      <c r="L20" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="M20" s="45" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3709,13 +3709,13 @@
       <c r="A21" s="18">
         <v>46</v>
       </c>
-      <c r="B21" s="97" t="s">
+      <c r="B21" s="93" t="s">
         <v>120</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="98" t="s">
+      <c r="D21" s="94" t="s">
         <v>121</v>
       </c>
       <c r="E21" s="22">
@@ -3733,88 +3733,88 @@
       <c r="I21" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="J21" s="32"/>
-      <c r="K21" s="99"/>
-      <c r="L21" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="M21" s="48" t="s">
+      <c r="J21" s="31"/>
+      <c r="K21" s="170"/>
+      <c r="L21" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="M21" s="45" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="34">
+      <c r="A22" s="32">
         <v>30</v>
       </c>
-      <c r="B22" s="100" t="s">
+      <c r="B22" s="95" t="s">
         <v>125</v>
       </c>
-      <c r="C22" s="101" t="s">
+      <c r="C22" s="96" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="102" t="s">
+      <c r="D22" s="97" t="s">
         <v>126</v>
       </c>
-      <c r="E22" s="103">
+      <c r="E22" s="98">
         <v>10</v>
       </c>
-      <c r="F22" s="104" t="s">
+      <c r="F22" s="99" t="s">
         <v>127</v>
       </c>
-      <c r="G22" s="105" t="s">
+      <c r="G22" s="100" t="s">
         <v>112</v>
       </c>
-      <c r="H22" s="101" t="s">
+      <c r="H22" s="96" t="s">
         <v>128</v>
       </c>
-      <c r="I22" s="106" t="s">
+      <c r="I22" s="101" t="s">
         <v>129</v>
       </c>
-      <c r="J22" s="38"/>
-      <c r="K22" s="99"/>
-      <c r="L22" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="M22" s="52" t="s">
+      <c r="J22" s="36"/>
+      <c r="K22" s="170"/>
+      <c r="L22" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="M22" s="49" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="40">
+      <c r="A23" s="38">
         <v>29</v>
       </c>
-      <c r="B23" s="95" t="s">
+      <c r="B23" s="91" t="s">
         <v>130</v>
       </c>
-      <c r="C23" s="54" t="s">
+      <c r="C23" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="96" t="s">
+      <c r="D23" s="92" t="s">
         <v>131</v>
       </c>
-      <c r="E23" s="56">
+      <c r="E23" s="53">
         <v>0</v>
       </c>
-      <c r="F23" s="57" t="s">
+      <c r="F23" s="54" t="s">
         <v>132</v>
       </c>
-      <c r="G23" s="58" t="s">
+      <c r="G23" s="55" t="s">
         <v>112</v>
       </c>
-      <c r="H23" s="54" t="s">
+      <c r="H23" s="51" t="s">
         <v>133</v>
       </c>
-      <c r="I23" s="79" t="s">
+      <c r="I23" s="75" t="s">
         <v>134</v>
       </c>
-      <c r="J23" s="61"/>
-      <c r="K23" s="47" t="s">
+      <c r="J23" s="58"/>
+      <c r="K23" s="169" t="s">
         <v>135</v>
       </c>
-      <c r="L23" s="107" t="s">
-        <v>19</v>
-      </c>
-      <c r="M23" s="107" t="s">
+      <c r="L23" s="102" t="s">
+        <v>19</v>
+      </c>
+      <c r="M23" s="102" t="s">
         <v>35</v>
       </c>
     </row>
@@ -3822,13 +3822,13 @@
       <c r="A24" s="18">
         <v>25</v>
       </c>
-      <c r="B24" s="97" t="s">
+      <c r="B24" s="93" t="s">
         <v>136</v>
       </c>
       <c r="C24" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="98" t="s">
+      <c r="D24" s="94" t="s">
         <v>137</v>
       </c>
       <c r="E24" s="22">
@@ -3843,17 +3843,17 @@
       <c r="H24" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="I24" s="63" t="s">
+      <c r="I24" s="60" t="s">
         <v>141</v>
       </c>
-      <c r="J24" s="32" t="s">
+      <c r="J24" s="31" t="s">
         <v>142</v>
       </c>
-      <c r="K24" s="99"/>
-      <c r="L24" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="M24" s="48" t="s">
+      <c r="K24" s="170"/>
+      <c r="L24" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="M24" s="45" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3861,106 +3861,106 @@
       <c r="A25" s="18">
         <v>68</v>
       </c>
-      <c r="B25" s="100" t="s">
+      <c r="B25" s="95" t="s">
         <v>143</v>
       </c>
-      <c r="C25" s="101" t="s">
+      <c r="C25" s="96" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="102" t="s">
+      <c r="D25" s="97" t="s">
         <v>144</v>
       </c>
-      <c r="E25" s="103">
+      <c r="E25" s="98">
         <v>277</v>
       </c>
-      <c r="F25" s="104" t="s">
+      <c r="F25" s="99" t="s">
         <v>145</v>
       </c>
-      <c r="G25" s="105" t="s">
+      <c r="G25" s="100" t="s">
         <v>112</v>
       </c>
-      <c r="H25" s="101" t="s">
+      <c r="H25" s="96" t="s">
         <v>146</v>
       </c>
-      <c r="I25" s="106" t="s">
+      <c r="I25" s="101" t="s">
         <v>147</v>
       </c>
-      <c r="J25" s="38"/>
-      <c r="K25" s="99"/>
-      <c r="L25" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="M25" s="48" t="s">
+      <c r="J25" s="36"/>
+      <c r="K25" s="170"/>
+      <c r="L25" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="M25" s="45" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="34">
+      <c r="A26" s="32">
         <v>23</v>
       </c>
-      <c r="B26" s="108" t="s">
+      <c r="B26" s="103" t="s">
         <v>148</v>
       </c>
-      <c r="C26" s="69" t="s">
+      <c r="C26" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="109" t="s">
+      <c r="D26" s="104" t="s">
         <v>137</v>
       </c>
-      <c r="E26" s="88">
+      <c r="E26" s="84">
         <v>37</v>
       </c>
-      <c r="F26" s="89">
+      <c r="F26" s="85">
         <v>1341</v>
       </c>
-      <c r="G26" s="90" t="s">
+      <c r="G26" s="86" t="s">
         <v>112</v>
       </c>
-      <c r="H26" s="110" t="s">
+      <c r="H26" s="105" t="s">
         <v>149</v>
       </c>
-      <c r="I26" s="91" t="s">
+      <c r="I26" s="87" t="s">
         <v>150</v>
       </c>
       <c r="J26" s="26"/>
-      <c r="K26" s="111"/>
-      <c r="L26" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="M26" s="52" t="s">
+      <c r="K26" s="176"/>
+      <c r="L26" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="M26" s="49" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="40">
+      <c r="A27" s="38">
         <v>22</v>
       </c>
-      <c r="B27" s="95" t="s">
+      <c r="B27" s="91" t="s">
         <v>151</v>
       </c>
-      <c r="C27" s="54" t="s">
+      <c r="C27" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="96" t="s">
+      <c r="D27" s="92" t="s">
         <v>137</v>
       </c>
-      <c r="E27" s="56">
+      <c r="E27" s="53">
         <v>18</v>
       </c>
-      <c r="F27" s="57">
+      <c r="F27" s="54">
         <v>1724</v>
       </c>
-      <c r="G27" s="58" t="s">
+      <c r="G27" s="55" t="s">
         <v>112</v>
       </c>
-      <c r="H27" s="54" t="s">
+      <c r="H27" s="51" t="s">
         <v>152</v>
       </c>
-      <c r="I27" s="79" t="s">
+      <c r="I27" s="75" t="s">
         <v>153</v>
       </c>
-      <c r="J27" s="61"/>
-      <c r="K27" s="47" t="s">
+      <c r="J27" s="58"/>
+      <c r="K27" s="169" t="s">
         <v>154</v>
       </c>
       <c r="L27" s="17" t="s">
@@ -3974,36 +3974,36 @@
       <c r="A28" s="18">
         <v>21</v>
       </c>
-      <c r="B28" s="100" t="s">
+      <c r="B28" s="95" t="s">
         <v>155</v>
       </c>
-      <c r="C28" s="101" t="s">
+      <c r="C28" s="96" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="102" t="s">
+      <c r="D28" s="97" t="s">
         <v>137</v>
       </c>
-      <c r="E28" s="103">
+      <c r="E28" s="98">
         <v>3</v>
       </c>
-      <c r="F28" s="104" t="s">
+      <c r="F28" s="99" t="s">
         <v>156</v>
       </c>
-      <c r="G28" s="105" t="s">
+      <c r="G28" s="100" t="s">
         <v>112</v>
       </c>
-      <c r="H28" s="112" t="s">
+      <c r="H28" s="106" t="s">
         <v>157</v>
       </c>
-      <c r="I28" s="113" t="s">
+      <c r="I28" s="107" t="s">
         <v>158</v>
       </c>
-      <c r="J28" s="38"/>
-      <c r="K28" s="99"/>
-      <c r="L28" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="M28" s="48" t="s">
+      <c r="J28" s="36"/>
+      <c r="K28" s="170"/>
+      <c r="L28" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="M28" s="45" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4011,108 +4011,108 @@
       <c r="A29" s="18">
         <v>28</v>
       </c>
-      <c r="B29" s="108" t="s">
+      <c r="B29" s="103" t="s">
         <v>159</v>
       </c>
-      <c r="C29" s="86" t="s">
+      <c r="C29" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="109" t="s">
+      <c r="D29" s="104" t="s">
         <v>160</v>
       </c>
-      <c r="E29" s="88">
+      <c r="E29" s="84">
         <v>4</v>
       </c>
-      <c r="F29" s="89" t="s">
+      <c r="F29" s="85" t="s">
         <v>161</v>
       </c>
-      <c r="G29" s="90" t="s">
+      <c r="G29" s="86" t="s">
         <v>112</v>
       </c>
-      <c r="H29" s="86" t="s">
+      <c r="H29" s="82" t="s">
         <v>162</v>
       </c>
-      <c r="I29" s="91" t="s">
+      <c r="I29" s="87" t="s">
         <v>163</v>
       </c>
       <c r="J29" s="26"/>
-      <c r="K29" s="99"/>
-      <c r="L29" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="M29" s="48" t="s">
+      <c r="K29" s="170"/>
+      <c r="L29" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="M29" s="45" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="34">
+      <c r="A30" s="32">
         <v>49</v>
       </c>
-      <c r="B30" s="114" t="s">
+      <c r="B30" s="108" t="s">
         <v>164</v>
       </c>
-      <c r="C30" s="69" t="s">
+      <c r="C30" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="D30" s="115" t="s">
+      <c r="D30" s="109" t="s">
         <v>165</v>
       </c>
-      <c r="E30" s="71">
+      <c r="E30" s="68">
         <v>7</v>
       </c>
-      <c r="F30" s="72">
+      <c r="F30" s="69">
         <v>1474</v>
       </c>
-      <c r="G30" s="73" t="s">
+      <c r="G30" s="70" t="s">
         <v>166</v>
       </c>
-      <c r="H30" s="69" t="s">
+      <c r="H30" s="66" t="s">
         <v>167</v>
       </c>
-      <c r="I30" s="116" t="s">
+      <c r="I30" s="110" t="s">
         <v>168</v>
       </c>
-      <c r="J30" s="76" t="s">
+      <c r="J30" s="73" t="s">
         <v>169</v>
       </c>
-      <c r="K30" s="111"/>
-      <c r="L30" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="M30" s="52" t="s">
+      <c r="K30" s="176"/>
+      <c r="L30" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="M30" s="49" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="15" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="40">
+      <c r="A31" s="38">
         <v>41</v>
       </c>
-      <c r="B31" s="117" t="s">
+      <c r="B31" s="111" t="s">
         <v>170</v>
       </c>
-      <c r="C31" s="54" t="s">
+      <c r="C31" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="D31" s="118" t="s">
+      <c r="D31" s="112" t="s">
         <v>171</v>
       </c>
-      <c r="E31" s="119">
-        <v>19</v>
-      </c>
-      <c r="F31" s="120" t="s">
+      <c r="E31" s="113">
+        <v>19</v>
+      </c>
+      <c r="F31" s="114" t="s">
         <v>172</v>
       </c>
-      <c r="G31" s="54" t="s">
+      <c r="G31" s="51" t="s">
         <v>173</v>
       </c>
-      <c r="H31" s="54" t="s">
+      <c r="H31" s="51" t="s">
         <v>174</v>
       </c>
-      <c r="I31" s="121" t="s">
+      <c r="I31" s="115" t="s">
         <v>175</v>
       </c>
-      <c r="J31" s="61"/>
-      <c r="K31" s="47" t="s">
+      <c r="J31" s="58"/>
+      <c r="K31" s="169" t="s">
         <v>176</v>
       </c>
       <c r="L31" s="17" t="s">
@@ -4126,19 +4126,19 @@
       <c r="A32" s="18">
         <v>50</v>
       </c>
-      <c r="B32" s="122" t="s">
+      <c r="B32" s="116" t="s">
         <v>177</v>
       </c>
       <c r="C32" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D32" s="118" t="s">
+      <c r="D32" s="112" t="s">
         <v>178</v>
       </c>
-      <c r="E32" s="123">
+      <c r="E32" s="117">
         <v>10</v>
       </c>
-      <c r="F32" s="124" t="s">
+      <c r="F32" s="118" t="s">
         <v>179</v>
       </c>
       <c r="G32" s="20" t="s">
@@ -4150,12 +4150,12 @@
       <c r="I32" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="J32" s="32"/>
-      <c r="K32" s="99"/>
-      <c r="L32" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="M32" s="48" t="s">
+      <c r="J32" s="31"/>
+      <c r="K32" s="170"/>
+      <c r="L32" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="M32" s="45" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4163,13 +4163,13 @@
       <c r="A33" s="18">
         <v>26</v>
       </c>
-      <c r="B33" s="97" t="s">
+      <c r="B33" s="93" t="s">
         <v>183</v>
       </c>
       <c r="C33" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D33" s="98" t="s">
+      <c r="D33" s="94" t="s">
         <v>184</v>
       </c>
       <c r="E33" s="22">
@@ -4181,88 +4181,88 @@
       <c r="G33" s="24" t="s">
         <v>185</v>
       </c>
-      <c r="H33" s="62" t="s">
+      <c r="H33" s="59" t="s">
         <v>186</v>
       </c>
       <c r="I33" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="J33" s="32"/>
-      <c r="K33" s="99"/>
-      <c r="L33" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="M33" s="48" t="s">
+      <c r="J33" s="31"/>
+      <c r="K33" s="170"/>
+      <c r="L33" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="M33" s="45" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="14.4" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="34">
+      <c r="A34" s="32">
         <v>40</v>
       </c>
-      <c r="B34" s="68" t="s">
+      <c r="B34" s="65" t="s">
         <v>188</v>
       </c>
-      <c r="C34" s="69" t="s">
+      <c r="C34" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="D34" s="70" t="s">
+      <c r="D34" s="67" t="s">
         <v>189</v>
       </c>
-      <c r="E34" s="71">
+      <c r="E34" s="68">
         <v>0</v>
       </c>
-      <c r="F34" s="72" t="s">
+      <c r="F34" s="69" t="s">
         <v>190</v>
       </c>
-      <c r="G34" s="69" t="s">
+      <c r="G34" s="66" t="s">
         <v>173</v>
       </c>
-      <c r="H34" s="74" t="s">
+      <c r="H34" s="71" t="s">
         <v>191</v>
       </c>
-      <c r="I34" s="94" t="s">
+      <c r="I34" s="90" t="s">
         <v>192</v>
       </c>
-      <c r="J34" s="76"/>
-      <c r="K34" s="111"/>
-      <c r="L34" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="M34" s="52" t="s">
+      <c r="J34" s="73"/>
+      <c r="K34" s="176"/>
+      <c r="L34" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="M34" s="49" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="40">
+      <c r="A35" s="38">
         <v>43</v>
       </c>
-      <c r="B35" s="117" t="s">
+      <c r="B35" s="111" t="s">
         <v>193</v>
       </c>
-      <c r="C35" s="54" t="s">
+      <c r="C35" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="D35" s="125" t="s">
+      <c r="D35" s="119" t="s">
         <v>194</v>
       </c>
-      <c r="E35" s="119">
+      <c r="E35" s="113">
         <v>34</v>
       </c>
-      <c r="F35" s="120" t="s">
+      <c r="F35" s="114" t="s">
         <v>195</v>
       </c>
-      <c r="G35" s="54" t="s">
+      <c r="G35" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="H35" s="54" t="s">
+      <c r="H35" s="51" t="s">
         <v>196</v>
       </c>
-      <c r="I35" s="121" t="s">
+      <c r="I35" s="115" t="s">
         <v>197</v>
       </c>
-      <c r="J35" s="61"/>
-      <c r="K35" s="47" t="s">
+      <c r="J35" s="58"/>
+      <c r="K35" s="169" t="s">
         <v>198</v>
       </c>
       <c r="L35" s="17" t="s">
@@ -4276,19 +4276,19 @@
       <c r="A36" s="18">
         <v>42</v>
       </c>
-      <c r="B36" s="122" t="s">
+      <c r="B36" s="116" t="s">
         <v>199</v>
       </c>
       <c r="C36" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="118" t="s">
+      <c r="D36" s="112" t="s">
         <v>200</v>
       </c>
-      <c r="E36" s="123">
+      <c r="E36" s="117">
         <v>10</v>
       </c>
-      <c r="F36" s="124" t="s">
+      <c r="F36" s="118" t="s">
         <v>201</v>
       </c>
       <c r="G36" s="20" t="s">
@@ -4300,12 +4300,12 @@
       <c r="I36" s="25" t="s">
         <v>203</v>
       </c>
-      <c r="J36" s="32"/>
-      <c r="K36" s="99"/>
-      <c r="L36" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="M36" s="48" t="s">
+      <c r="J36" s="31"/>
+      <c r="K36" s="170"/>
+      <c r="L36" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="M36" s="45" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4313,13 +4313,13 @@
       <c r="A37" s="18">
         <v>27</v>
       </c>
-      <c r="B37" s="97" t="s">
+      <c r="B37" s="93" t="s">
         <v>204</v>
       </c>
       <c r="C37" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D37" s="98" t="s">
+      <c r="D37" s="94" t="s">
         <v>184</v>
       </c>
       <c r="E37" s="22">
@@ -4337,28 +4337,28 @@
       <c r="I37" s="25" t="s">
         <v>207</v>
       </c>
-      <c r="J37" s="61" t="s">
+      <c r="J37" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="K37" s="99"/>
-      <c r="L37" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="M37" s="48" t="s">
+      <c r="K37" s="170"/>
+      <c r="L37" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="M37" s="45" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="34">
+      <c r="A38" s="32">
         <v>47</v>
       </c>
-      <c r="B38" s="97" t="s">
+      <c r="B38" s="93" t="s">
         <v>208</v>
       </c>
       <c r="C38" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D38" s="98" t="s">
+      <c r="D38" s="94" t="s">
         <v>209</v>
       </c>
       <c r="E38" s="22">
@@ -4376,45 +4376,45 @@
       <c r="I38" s="25" t="s">
         <v>212</v>
       </c>
-      <c r="J38" s="32"/>
-      <c r="K38" s="99"/>
-      <c r="L38" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="M38" s="52" t="s">
+      <c r="J38" s="31"/>
+      <c r="K38" s="170"/>
+      <c r="L38" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="M38" s="49" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="14.4" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="40">
+      <c r="A39" s="38">
         <v>18</v>
       </c>
-      <c r="B39" s="117" t="s">
+      <c r="B39" s="111" t="s">
         <v>213</v>
       </c>
-      <c r="C39" s="54" t="s">
+      <c r="C39" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="D39" s="125" t="s">
+      <c r="D39" s="119" t="s">
         <v>214</v>
       </c>
-      <c r="E39" s="119">
+      <c r="E39" s="113">
         <v>143</v>
       </c>
-      <c r="F39" s="120" t="s">
+      <c r="F39" s="114" t="s">
         <v>215</v>
       </c>
-      <c r="G39" s="54" t="s">
+      <c r="G39" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="H39" s="54" t="s">
+      <c r="H39" s="51" t="s">
         <v>216</v>
       </c>
-      <c r="I39" s="121" t="s">
+      <c r="I39" s="115" t="s">
         <v>217</v>
       </c>
-      <c r="J39" s="61"/>
-      <c r="K39" s="47" t="s">
+      <c r="J39" s="58"/>
+      <c r="K39" s="169" t="s">
         <v>218</v>
       </c>
       <c r="L39" s="17" t="s">
@@ -4428,19 +4428,19 @@
       <c r="A40" s="18">
         <v>11</v>
       </c>
-      <c r="B40" s="122" t="s">
+      <c r="B40" s="116" t="s">
         <v>219</v>
       </c>
       <c r="C40" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D40" s="118" t="s">
+      <c r="D40" s="112" t="s">
         <v>214</v>
       </c>
-      <c r="E40" s="123">
+      <c r="E40" s="117">
         <v>150</v>
       </c>
-      <c r="F40" s="124">
+      <c r="F40" s="118">
         <v>1650</v>
       </c>
       <c r="G40" s="20" t="s">
@@ -4452,12 +4452,12 @@
       <c r="I40" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="J40" s="32"/>
-      <c r="K40" s="99"/>
-      <c r="L40" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="M40" s="48" t="s">
+      <c r="J40" s="31"/>
+      <c r="K40" s="170"/>
+      <c r="L40" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="M40" s="45" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4465,13 +4465,13 @@
       <c r="A41" s="18">
         <v>60</v>
       </c>
-      <c r="B41" s="97" t="s">
+      <c r="B41" s="93" t="s">
         <v>222</v>
       </c>
       <c r="C41" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D41" s="98" t="s">
+      <c r="D41" s="94" t="s">
         <v>22</v>
       </c>
       <c r="E41" s="22">
@@ -4489,12 +4489,12 @@
       <c r="I41" s="25" t="s">
         <v>225</v>
       </c>
-      <c r="J41" s="32"/>
-      <c r="K41" s="99"/>
-      <c r="L41" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="M41" s="48" t="s">
+      <c r="J41" s="31"/>
+      <c r="K41" s="170"/>
+      <c r="L41" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="M41" s="45" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4502,13 +4502,13 @@
       <c r="A42" s="18">
         <v>55</v>
       </c>
-      <c r="B42" s="97" t="s">
+      <c r="B42" s="93" t="s">
         <v>226</v>
       </c>
       <c r="C42" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D42" s="98" t="s">
+      <c r="D42" s="94" t="s">
         <v>227</v>
       </c>
       <c r="E42" s="22">
@@ -4527,11 +4527,11 @@
         <v>230</v>
       </c>
       <c r="J42" s="26"/>
-      <c r="K42" s="99"/>
-      <c r="L42" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="M42" s="48" t="s">
+      <c r="K42" s="170"/>
+      <c r="L42" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="M42" s="45" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4539,91 +4539,91 @@
       <c r="A43" s="18">
         <v>61</v>
       </c>
-      <c r="B43" s="85" t="s">
+      <c r="B43" s="81" t="s">
         <v>231</v>
       </c>
-      <c r="C43" s="86" t="s">
+      <c r="C43" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="D43" s="87" t="s">
+      <c r="D43" s="83" t="s">
         <v>232</v>
       </c>
-      <c r="E43" s="88">
+      <c r="E43" s="84">
         <v>11</v>
       </c>
-      <c r="F43" s="89">
+      <c r="F43" s="85">
         <v>1540</v>
       </c>
-      <c r="G43" s="86" t="s">
+      <c r="G43" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="H43" s="86" t="s">
+      <c r="H43" s="82" t="s">
         <v>233</v>
       </c>
-      <c r="I43" s="91" t="s">
+      <c r="I43" s="87" t="s">
         <v>234</v>
       </c>
       <c r="J43" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="K43" s="99"/>
-      <c r="L43" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="M43" s="52" t="s">
+      <c r="K43" s="170"/>
+      <c r="L43" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="M43" s="49" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="14.4" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="34">
+      <c r="A44" s="32">
         <v>20</v>
       </c>
-      <c r="B44" s="126" t="s">
+      <c r="B44" s="120" t="s">
         <v>235</v>
       </c>
-      <c r="C44" s="69" t="s">
+      <c r="C44" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="D44" s="127" t="s">
+      <c r="D44" s="121" t="s">
         <v>236</v>
       </c>
-      <c r="E44" s="128">
+      <c r="E44" s="122">
         <v>21</v>
       </c>
-      <c r="F44" s="129" t="s">
+      <c r="F44" s="123" t="s">
         <v>237</v>
       </c>
-      <c r="G44" s="69" t="s">
+      <c r="G44" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="H44" s="69" t="s">
+      <c r="H44" s="66" t="s">
         <v>238</v>
       </c>
-      <c r="I44" s="91" t="s">
+      <c r="I44" s="87" t="s">
         <v>239</v>
       </c>
-      <c r="J44" s="32" t="s">
+      <c r="J44" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="K44" s="130"/>
-      <c r="L44" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="M44" s="48" t="s">
+      <c r="K44" s="124"/>
+      <c r="L44" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="M44" s="45" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="14.4" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="40">
+      <c r="A45" s="38">
         <v>56</v>
       </c>
-      <c r="B45" s="97" t="s">
+      <c r="B45" s="93" t="s">
         <v>240</v>
       </c>
-      <c r="C45" s="69" t="s">
+      <c r="C45" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="D45" s="98" t="s">
+      <c r="D45" s="94" t="s">
         <v>241</v>
       </c>
       <c r="E45" s="22">
@@ -4638,52 +4638,52 @@
       <c r="H45" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="I45" s="82" t="s">
+      <c r="I45" s="78" t="s">
         <v>244</v>
       </c>
-      <c r="J45" s="32"/>
-      <c r="K45" s="131"/>
-      <c r="L45" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="M45" s="48" t="s">
+      <c r="J45" s="31"/>
+      <c r="K45" s="177"/>
+      <c r="L45" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="M45" s="45" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="14.4" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="132">
+      <c r="A46" s="125">
         <v>37</v>
       </c>
-      <c r="B46" s="68" t="s">
+      <c r="B46" s="65" t="s">
         <v>245</v>
       </c>
-      <c r="C46" s="133" t="s">
+      <c r="C46" s="126" t="s">
         <v>21</v>
       </c>
-      <c r="D46" s="70" t="s">
+      <c r="D46" s="67" t="s">
         <v>246</v>
       </c>
-      <c r="E46" s="71">
+      <c r="E46" s="68">
         <v>20</v>
       </c>
-      <c r="F46" s="72" t="s">
+      <c r="F46" s="69" t="s">
         <v>247</v>
       </c>
-      <c r="G46" s="73" t="s">
+      <c r="G46" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="H46" s="69" t="s">
+      <c r="H46" s="66" t="s">
         <v>248</v>
       </c>
-      <c r="I46" s="94" t="s">
+      <c r="I46" s="90" t="s">
         <v>249</v>
       </c>
-      <c r="J46" s="76"/>
-      <c r="K46" s="134"/>
-      <c r="L46" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="M46" s="52" t="s">
+      <c r="J46" s="73"/>
+      <c r="K46" s="178"/>
+      <c r="L46" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="M46" s="49" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4691,32 +4691,32 @@
       <c r="A47" s="18">
         <v>35</v>
       </c>
-      <c r="B47" s="117" t="s">
+      <c r="B47" s="111" t="s">
         <v>250</v>
       </c>
-      <c r="C47" s="54" t="s">
+      <c r="C47" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="D47" s="125" t="s">
+      <c r="D47" s="119" t="s">
         <v>251</v>
       </c>
-      <c r="E47" s="119">
+      <c r="E47" s="113">
         <v>8</v>
       </c>
-      <c r="F47" s="120" t="s">
+      <c r="F47" s="114" t="s">
         <v>252</v>
       </c>
-      <c r="G47" s="135" t="s">
+      <c r="G47" s="127" t="s">
         <v>253</v>
       </c>
-      <c r="H47" s="54" t="s">
+      <c r="H47" s="51" t="s">
         <v>254</v>
       </c>
-      <c r="I47" s="121" t="s">
+      <c r="I47" s="115" t="s">
         <v>255</v>
       </c>
-      <c r="J47" s="61"/>
-      <c r="K47" s="47" t="s">
+      <c r="J47" s="58"/>
+      <c r="K47" s="169" t="s">
         <v>256</v>
       </c>
       <c r="L47" s="17" t="s">
@@ -4730,19 +4730,19 @@
       <c r="A48" s="18">
         <v>39</v>
       </c>
-      <c r="B48" s="122" t="s">
+      <c r="B48" s="116" t="s">
         <v>257</v>
       </c>
       <c r="C48" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D48" s="118" t="s">
+      <c r="D48" s="112" t="s">
         <v>258</v>
       </c>
-      <c r="E48" s="123">
+      <c r="E48" s="117">
         <v>187</v>
       </c>
-      <c r="F48" s="124" t="s">
+      <c r="F48" s="118" t="s">
         <v>259</v>
       </c>
       <c r="G48" s="20" t="s">
@@ -4754,12 +4754,12 @@
       <c r="I48" s="25" t="s">
         <v>261</v>
       </c>
-      <c r="J48" s="32"/>
-      <c r="K48" s="99"/>
-      <c r="L48" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="M48" s="48" t="s">
+      <c r="J48" s="31"/>
+      <c r="K48" s="170"/>
+      <c r="L48" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="M48" s="45" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4767,36 +4767,36 @@
       <c r="A49" s="18">
         <v>34</v>
       </c>
-      <c r="B49" s="85" t="s">
+      <c r="B49" s="81" t="s">
         <v>262</v>
       </c>
-      <c r="C49" s="86" t="s">
+      <c r="C49" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="D49" s="87" t="s">
+      <c r="D49" s="83" t="s">
         <v>263</v>
       </c>
-      <c r="E49" s="88">
+      <c r="E49" s="84">
         <v>4</v>
       </c>
-      <c r="F49" s="89">
+      <c r="F49" s="85">
         <v>1144</v>
       </c>
-      <c r="G49" s="86" t="s">
+      <c r="G49" s="82" t="s">
         <v>264</v>
       </c>
-      <c r="H49" s="86" t="s">
+      <c r="H49" s="82" t="s">
         <v>265</v>
       </c>
-      <c r="I49" s="91" t="s">
+      <c r="I49" s="87" t="s">
         <v>266</v>
       </c>
       <c r="J49" s="26"/>
-      <c r="K49" s="99"/>
-      <c r="L49" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="M49" s="48" t="s">
+      <c r="K49" s="170"/>
+      <c r="L49" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="M49" s="45" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4804,13 +4804,13 @@
       <c r="A50" s="18">
         <v>48</v>
       </c>
-      <c r="B50" s="97" t="s">
+      <c r="B50" s="93" t="s">
         <v>267</v>
       </c>
       <c r="C50" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D50" s="98" t="s">
+      <c r="D50" s="94" t="s">
         <v>268</v>
       </c>
       <c r="E50" s="22">
@@ -4828,14 +4828,14 @@
       <c r="I50" s="25" t="s">
         <v>271</v>
       </c>
-      <c r="J50" s="61" t="s">
+      <c r="J50" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="K50" s="99"/>
-      <c r="L50" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="M50" s="48" t="s">
+      <c r="K50" s="170"/>
+      <c r="L50" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="M50" s="45" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4843,36 +4843,36 @@
       <c r="A51" s="18">
         <v>24</v>
       </c>
-      <c r="B51" s="68" t="s">
+      <c r="B51" s="65" t="s">
         <v>272</v>
       </c>
-      <c r="C51" s="69" t="s">
+      <c r="C51" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="D51" s="70" t="s">
+      <c r="D51" s="67" t="s">
         <v>273</v>
       </c>
-      <c r="E51" s="71">
+      <c r="E51" s="68">
         <v>169</v>
       </c>
-      <c r="F51" s="72" t="s">
+      <c r="F51" s="69" t="s">
         <v>100</v>
       </c>
-      <c r="G51" s="69" t="s">
+      <c r="G51" s="66" t="s">
         <v>173</v>
       </c>
-      <c r="H51" s="69" t="s">
+      <c r="H51" s="66" t="s">
         <v>274</v>
       </c>
-      <c r="I51" s="75" t="s">
+      <c r="I51" s="72" t="s">
         <v>275</v>
       </c>
-      <c r="J51" s="76"/>
-      <c r="K51" s="99"/>
-      <c r="L51" s="78" t="s">
-        <v>19</v>
-      </c>
-      <c r="M51" s="78" t="s">
+      <c r="J51" s="73"/>
+      <c r="K51" s="170"/>
+      <c r="L51" s="74" t="s">
+        <v>19</v>
+      </c>
+      <c r="M51" s="74" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4880,38 +4880,38 @@
       <c r="A52" s="18">
         <v>33</v>
       </c>
-      <c r="B52" s="136" t="s">
+      <c r="B52" s="128" t="s">
         <v>276</v>
       </c>
-      <c r="C52" s="137" t="s">
+      <c r="C52" s="129" t="s">
         <v>14</v>
       </c>
-      <c r="D52" s="138" t="s">
+      <c r="D52" s="130" t="s">
         <v>277</v>
       </c>
-      <c r="E52" s="139">
+      <c r="E52" s="131">
         <v>180</v>
       </c>
-      <c r="F52" s="140" t="s">
+      <c r="F52" s="132" t="s">
         <v>31</v>
       </c>
-      <c r="G52" s="137" t="s">
+      <c r="G52" s="129" t="s">
         <v>185</v>
       </c>
-      <c r="H52" s="137" t="s">
+      <c r="H52" s="129" t="s">
         <v>278</v>
       </c>
-      <c r="I52" s="141" t="s">
+      <c r="I52" s="133" t="s">
         <v>279</v>
       </c>
-      <c r="J52" s="142"/>
-      <c r="K52" s="47" t="s">
+      <c r="J52" s="134"/>
+      <c r="K52" s="169" t="s">
         <v>280</v>
       </c>
-      <c r="L52" s="80" t="s">
-        <v>19</v>
-      </c>
-      <c r="M52" s="80" t="s">
+      <c r="L52" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="M52" s="76" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4919,106 +4919,106 @@
       <c r="A53" s="18">
         <v>32</v>
       </c>
-      <c r="B53" s="85" t="s">
+      <c r="B53" s="81" t="s">
         <v>281</v>
       </c>
-      <c r="C53" s="86" t="s">
+      <c r="C53" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="D53" s="87" t="s">
+      <c r="D53" s="83" t="s">
         <v>282</v>
       </c>
-      <c r="E53" s="88">
+      <c r="E53" s="84">
         <v>166</v>
       </c>
-      <c r="F53" s="89">
+      <c r="F53" s="85">
         <v>1239</v>
       </c>
-      <c r="G53" s="86" t="s">
+      <c r="G53" s="82" t="s">
         <v>185</v>
       </c>
-      <c r="H53" s="86" t="s">
+      <c r="H53" s="82" t="s">
         <v>283</v>
       </c>
-      <c r="I53" s="91" t="s">
+      <c r="I53" s="87" t="s">
         <v>284</v>
       </c>
       <c r="J53" s="26"/>
-      <c r="K53" s="33"/>
-      <c r="L53" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="M53" s="48" t="s">
+      <c r="K53" s="171"/>
+      <c r="L53" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="M53" s="45" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="14.4" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="34">
+      <c r="A54" s="32">
         <v>31</v>
       </c>
-      <c r="B54" s="85" t="s">
+      <c r="B54" s="81" t="s">
         <v>285</v>
       </c>
-      <c r="C54" s="69" t="s">
+      <c r="C54" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="D54" s="70" t="s">
+      <c r="D54" s="67" t="s">
         <v>286</v>
       </c>
-      <c r="E54" s="71">
+      <c r="E54" s="68">
         <v>158</v>
       </c>
-      <c r="F54" s="72" t="s">
+      <c r="F54" s="69" t="s">
         <v>287</v>
       </c>
-      <c r="G54" s="69" t="s">
+      <c r="G54" s="66" t="s">
         <v>185</v>
       </c>
-      <c r="H54" s="69" t="s">
+      <c r="H54" s="66" t="s">
         <v>288</v>
       </c>
-      <c r="I54" s="94" t="s">
+      <c r="I54" s="90" t="s">
         <v>289</v>
       </c>
-      <c r="J54" s="76"/>
-      <c r="K54" s="77"/>
-      <c r="L54" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="M54" s="52" t="s">
+      <c r="J54" s="73"/>
+      <c r="K54" s="172"/>
+      <c r="L54" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="M54" s="49" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="15" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="40">
+      <c r="A55" s="38">
         <v>66</v>
       </c>
-      <c r="B55" s="143" t="s">
+      <c r="B55" s="135" t="s">
         <v>290</v>
       </c>
-      <c r="C55" s="121" t="s">
+      <c r="C55" s="115" t="s">
         <v>21</v>
       </c>
-      <c r="D55" s="55" t="s">
+      <c r="D55" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="E55" s="55">
+      <c r="E55" s="52">
         <v>127</v>
       </c>
-      <c r="F55" s="144" t="s">
+      <c r="F55" s="136" t="s">
         <v>291</v>
       </c>
-      <c r="G55" s="42" t="s">
+      <c r="G55" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="H55" s="145" t="s">
+      <c r="H55" s="137" t="s">
         <v>292</v>
       </c>
-      <c r="I55" s="60" t="s">
+      <c r="I55" s="57" t="s">
         <v>293</v>
       </c>
-      <c r="J55" s="146"/>
-      <c r="K55" s="147" t="s">
+      <c r="J55" s="138"/>
+      <c r="K55" s="173" t="s">
         <v>294</v>
       </c>
       <c r="L55" s="17" t="s">
@@ -5032,36 +5032,36 @@
       <c r="A56" s="18">
         <v>8</v>
       </c>
-      <c r="B56" s="148" t="s">
+      <c r="B56" s="139" t="s">
         <v>295</v>
       </c>
       <c r="C56" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="D56" s="30" t="s">
+      <c r="D56" s="29" t="s">
         <v>296</v>
       </c>
-      <c r="E56" s="30">
+      <c r="E56" s="29">
         <v>2</v>
       </c>
-      <c r="F56" s="31" t="s">
+      <c r="F56" s="30" t="s">
         <v>297</v>
       </c>
       <c r="G56" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="H56" s="149" t="s">
+      <c r="H56" s="140" t="s">
         <v>298</v>
       </c>
-      <c r="I56" s="150" t="s">
+      <c r="I56" s="141" t="s">
         <v>299</v>
       </c>
-      <c r="J56" s="151"/>
-      <c r="K56" s="152"/>
-      <c r="L56" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="M56" s="52" t="s">
+      <c r="J56" s="142"/>
+      <c r="K56" s="174"/>
+      <c r="L56" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="M56" s="49" t="s">
         <v>19</v>
       </c>
     </row>
@@ -5069,36 +5069,36 @@
       <c r="A57" s="18">
         <v>12</v>
       </c>
-      <c r="B57" s="148" t="s">
+      <c r="B57" s="139" t="s">
         <v>300</v>
       </c>
       <c r="C57" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="D57" s="153" t="s">
+      <c r="D57" s="143" t="s">
         <v>301</v>
       </c>
-      <c r="E57" s="30">
+      <c r="E57" s="29">
         <v>70</v>
       </c>
-      <c r="F57" s="31" t="s">
+      <c r="F57" s="30" t="s">
         <v>302</v>
       </c>
       <c r="G57" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="H57" s="154" t="s">
+      <c r="H57" s="144" t="s">
         <v>303</v>
       </c>
-      <c r="I57" s="94" t="s">
+      <c r="I57" s="90" t="s">
         <v>304</v>
       </c>
-      <c r="J57" s="155"/>
-      <c r="K57" s="156"/>
-      <c r="L57" s="78" t="s">
-        <v>19</v>
-      </c>
-      <c r="M57" s="78" t="s">
+      <c r="J57" s="145"/>
+      <c r="K57" s="175"/>
+      <c r="L57" s="74" t="s">
+        <v>19</v>
+      </c>
+      <c r="M57" s="74" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5106,7 +5106,7 @@
       <c r="A58" s="18">
         <v>57</v>
       </c>
-      <c r="B58" s="157" t="s">
+      <c r="B58" s="146" t="s">
         <v>305</v>
       </c>
       <c r="C58" s="20" t="s">
@@ -5130,16 +5130,16 @@
       <c r="I58" s="25" t="s">
         <v>308</v>
       </c>
-      <c r="J58" s="61" t="s">
+      <c r="J58" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="K58" s="47" t="s">
+      <c r="K58" s="169" t="s">
         <v>309</v>
       </c>
-      <c r="L58" s="80" t="s">
-        <v>19</v>
-      </c>
-      <c r="M58" s="80" t="s">
+      <c r="L58" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="M58" s="76" t="s">
         <v>19</v>
       </c>
     </row>
@@ -5147,7 +5147,7 @@
       <c r="A59" s="18">
         <v>10</v>
       </c>
-      <c r="B59" s="157" t="s">
+      <c r="B59" s="146" t="s">
         <v>310</v>
       </c>
       <c r="C59" s="20" t="s">
@@ -5171,14 +5171,14 @@
       <c r="I59" s="25" t="s">
         <v>313</v>
       </c>
-      <c r="J59" s="61" t="s">
+      <c r="J59" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="K59" s="99"/>
-      <c r="L59" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="M59" s="48" t="s">
+      <c r="K59" s="170"/>
+      <c r="L59" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="M59" s="45" t="s">
         <v>19</v>
       </c>
     </row>
@@ -5186,105 +5186,105 @@
       <c r="A60" s="18">
         <v>51</v>
       </c>
-      <c r="B60" s="108" t="s">
+      <c r="B60" s="103" t="s">
         <v>314</v>
       </c>
-      <c r="C60" s="86" t="s">
+      <c r="C60" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="D60" s="87" t="s">
+      <c r="D60" s="83" t="s">
         <v>315</v>
       </c>
-      <c r="E60" s="88">
+      <c r="E60" s="84">
         <v>21</v>
       </c>
-      <c r="F60" s="158" t="s">
+      <c r="F60" s="147" t="s">
         <v>316</v>
       </c>
-      <c r="G60" s="90" t="s">
+      <c r="G60" s="86" t="s">
         <v>317</v>
       </c>
-      <c r="H60" s="159" t="s">
+      <c r="H60" s="148" t="s">
         <v>318</v>
       </c>
-      <c r="I60" s="160" t="s">
+      <c r="I60" s="149" t="s">
         <v>319</v>
       </c>
       <c r="J60" s="26"/>
-      <c r="K60" s="161" t="s">
+      <c r="K60" s="150" t="s">
         <v>320</v>
       </c>
-      <c r="L60" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="M60" s="52" t="s">
+      <c r="L60" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="M60" s="49" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="14.4" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="162">
+      <c r="A61" s="151">
         <v>65</v>
       </c>
-      <c r="B61" s="163" t="s">
+      <c r="B61" s="152" t="s">
         <v>321</v>
       </c>
-      <c r="C61" s="164" t="s">
+      <c r="C61" s="153" t="s">
         <v>21</v>
       </c>
-      <c r="D61" s="165" t="s">
+      <c r="D61" s="154" t="s">
         <v>22</v>
       </c>
-      <c r="E61" s="166">
+      <c r="E61" s="155">
         <v>116</v>
       </c>
-      <c r="F61" s="167" t="s">
+      <c r="F61" s="156" t="s">
         <v>322</v>
       </c>
-      <c r="G61" s="168" t="s">
+      <c r="G61" s="157" t="s">
         <v>323</v>
       </c>
-      <c r="H61" s="164" t="s">
+      <c r="H61" s="153" t="s">
         <v>324</v>
       </c>
-      <c r="I61" s="169" t="s">
+      <c r="I61" s="158" t="s">
         <v>325</v>
       </c>
-      <c r="J61" s="170"/>
-      <c r="K61" s="171"/>
-      <c r="L61" s="172" t="s">
+      <c r="J61" s="159"/>
+      <c r="K61" s="160"/>
+      <c r="L61" s="161" t="s">
         <v>326</v>
       </c>
-      <c r="M61" s="172" t="s">
+      <c r="M61" s="161" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K62" s="173"/>
+      <c r="K62" s="162"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K63" s="173"/>
+      <c r="K63" s="162"/>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K64" s="174"/>
+      <c r="K64" s="163"/>
     </row>
     <row r="65" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C65" s="175"/>
-      <c r="F65" s="176"/>
-      <c r="G65" s="177"/>
-      <c r="H65" s="175"/>
-      <c r="I65" s="178"/>
-      <c r="J65" s="179"/>
-      <c r="K65" s="173"/>
+      <c r="C65" s="164"/>
+      <c r="F65" s="165"/>
+      <c r="G65" s="166"/>
+      <c r="H65" s="164"/>
+      <c r="I65" s="167"/>
+      <c r="J65" s="168"/>
+      <c r="K65" s="162"/>
     </row>
     <row r="66" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="J66" s="179"/>
-      <c r="K66" s="173"/>
+      <c r="J66" s="168"/>
+      <c r="K66" s="162"/>
     </row>
     <row r="67" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="K67" s="173"/>
+      <c r="K67" s="162"/>
     </row>
     <row r="68" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="K68" s="173"/>
+      <c r="K68" s="162"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:M61" xr:uid="{8B77CC5D-50A3-45ED-BF74-80ABEB93B7B1}">
@@ -5303,6 +5303,12 @@
     </filterColumn>
   </autoFilter>
   <mergeCells count="16">
+    <mergeCell ref="K19:K22"/>
+    <mergeCell ref="K3:K5"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="K9:K12"/>
+    <mergeCell ref="K13:K16"/>
+    <mergeCell ref="K17:K18"/>
     <mergeCell ref="K47:K51"/>
     <mergeCell ref="K52:K54"/>
     <mergeCell ref="K55:K57"/>
@@ -5313,12 +5319,6 @@
     <mergeCell ref="K35:K38"/>
     <mergeCell ref="K39:K43"/>
     <mergeCell ref="K45:K46"/>
-    <mergeCell ref="K3:K5"/>
-    <mergeCell ref="K6:K8"/>
-    <mergeCell ref="K9:K12"/>
-    <mergeCell ref="K13:K16"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="K19:K22"/>
   </mergeCells>
   <conditionalFormatting sqref="L3:M61">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">

</xml_diff>